<commit_message>
Commit "Register test case files"
</commit_message>
<xml_diff>
--- a/Dsalgo/src/test/resources/Exceldata/Login.xlsx
+++ b/Dsalgo/src/test/resources/Exceldata/Login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurbax Gill\git\justautomation\Dsalgo\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E612FD7-D966-48CE-A4C4-4F9A19C74546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5516AC1C-03C0-4D3B-A1DE-5D6E04A2222A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="3120" windowWidth="15996" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Numpysdet84</t>
-  </si>
-  <si>
-    <t>user</t>
   </si>
   <si>
     <t>Invalid Username and Password</t>
@@ -415,7 +412,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -441,11 +438,9 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -453,21 +448,21 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -475,10 +470,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -503,90 +498,90 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit -m "added DS files"
</commit_message>
<xml_diff>
--- a/Dsalgo/src/test/resources/Exceldata/Login.xlsx
+++ b/Dsalgo/src/test/resources/Exceldata/Login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurbax Gill\git\justautomation\Dsalgo\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5516AC1C-03C0-4D3B-A1DE-5D6E04A2222A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC81B9-BCCC-4F98-8B94-DD80CA41C6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="3120" windowWidth="15996" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Numpysdet84</t>
   </si>
   <si>
-    <t>Invalid Username and Password</t>
-  </si>
-  <si>
     <t>sdet84batch</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
   </si>
   <si>
     <t>Numpysdet86</t>
-  </si>
-  <si>
-    <t>sdet86batch</t>
   </si>
   <si>
     <t>pythonCode</t>
@@ -136,6 +130,18 @@
   </si>
   <si>
     <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>print("hello")</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>NameError: name 'hello' is not defined on line</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -420,10 +426,12 @@
     <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="28.109375" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="25" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,47 +441,94 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -489,99 +544,102 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" customWidth="1"/>
+    <col min="1" max="1" width="219" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit -m "commit list files"
</commit_message>
<xml_diff>
--- a/Dsalgo/src/test/resources/Exceldata/Login.xlsx
+++ b/Dsalgo/src/test/resources/Exceldata/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurbax Gill\git\justautomation\Dsalgo\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC81B9-BCCC-4F98-8B94-DD80CA41C6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBEFCEE-83BD-43CC-8C7D-3906BC04404C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -193,13 +193,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -426,7 +432,7 @@
     <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="28.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="129.77734375" customWidth="1"/>
     <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
     <col min="6" max="25" width="8.6640625" customWidth="1"/>
   </cols>
@@ -529,6 +535,23 @@
       </c>
       <c r="E6" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -544,8 +567,8 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -579,7 +602,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -587,7 +610,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -595,7 +618,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -603,7 +626,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -611,7 +634,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">

</xml_diff>